<commit_message>
Updated main file ready for AI utilization
</commit_message>
<xml_diff>
--- a/main/MilitaryTactics.xlsx
+++ b/main/MilitaryTactics.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\studentgvsc\Documents\Mentorship2020\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F01165-DA3B-4324-876E-9C0BE2D8A182}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35B4411-DFCE-48FA-A2A8-F1550CCE2652}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="MatrixForPython" sheetId="2" r:id="rId1"/>
+    <sheet name="Matrix for Python" sheetId="3" r:id="rId1"/>
     <sheet name="MilitaryTactics" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -366,333 +366,333 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2607E7BB-C004-44AA-8DC2-006BC49BA4E2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EB7B92-D441-486F-8C97-99D4DEFFD492}">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="3">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6">
-        <v>1</v>
-      </c>
-      <c r="D1" s="6">
-        <v>-1</v>
-      </c>
-      <c r="E1" s="6">
-        <v>1</v>
-      </c>
-      <c r="F1" s="6">
-        <v>-1</v>
-      </c>
-      <c r="G1" s="6">
-        <v>0</v>
-      </c>
-      <c r="H1" s="6">
-        <v>-1</v>
-      </c>
-      <c r="I1" s="6">
-        <v>-1</v>
-      </c>
-      <c r="J1" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
-        <v>-1</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6">
-        <v>-1</v>
-      </c>
-      <c r="E2" s="6">
-        <v>1</v>
-      </c>
-      <c r="F2" s="6">
-        <v>-1</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6">
-        <v>-1</v>
-      </c>
-      <c r="I2" s="6">
-        <v>-1</v>
-      </c>
-      <c r="J2" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>-1</v>
-      </c>
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>-1</v>
-      </c>
-      <c r="E3" s="6">
-        <v>1</v>
-      </c>
-      <c r="F3" s="6">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6">
-        <v>-1</v>
-      </c>
-      <c r="I3" s="6">
-        <v>-1</v>
-      </c>
-      <c r="J3" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>-1</v>
-      </c>
-      <c r="F4" s="6">
-        <v>1</v>
-      </c>
-      <c r="G4" s="6">
-        <v>1</v>
-      </c>
-      <c r="H4" s="6">
-        <v>1</v>
-      </c>
-      <c r="I4" s="6">
-        <v>1</v>
-      </c>
-      <c r="J4" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>-1</v>
-      </c>
-      <c r="B5" s="6">
-        <v>-1</v>
-      </c>
-      <c r="C5" s="6">
-        <v>-1</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>1</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
-        <v>-1</v>
-      </c>
-      <c r="I5" s="6">
-        <v>-1</v>
-      </c>
-      <c r="J5" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>1</v>
-      </c>
-      <c r="B6" s="6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="6">
-        <v>-1</v>
-      </c>
-      <c r="D6" s="6">
-        <v>-1</v>
-      </c>
-      <c r="E6" s="6">
-        <v>-1</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6">
-        <v>1</v>
-      </c>
-      <c r="H6" s="6">
-        <v>1</v>
-      </c>
-      <c r="I6" s="6">
-        <v>1</v>
-      </c>
-      <c r="J6" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>0</v>
-      </c>
-      <c r="B7" s="6">
-        <v>0</v>
-      </c>
-      <c r="C7" s="6">
-        <v>0</v>
-      </c>
-      <c r="D7" s="6">
-        <v>-1</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6">
-        <v>-1</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6">
-        <v>-1</v>
-      </c>
-      <c r="I7" s="6">
-        <v>0</v>
-      </c>
-      <c r="J7" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>1</v>
-      </c>
-      <c r="B8" s="6">
-        <v>1</v>
-      </c>
-      <c r="C8" s="6">
-        <v>1</v>
-      </c>
-      <c r="D8" s="6">
-        <v>-1</v>
-      </c>
-      <c r="E8" s="6">
-        <v>1</v>
-      </c>
-      <c r="F8" s="6">
-        <v>-1</v>
-      </c>
-      <c r="G8" s="6">
-        <v>1</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0</v>
-      </c>
-      <c r="I8" s="7">
-        <v>0</v>
-      </c>
-      <c r="J8" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>1</v>
-      </c>
-      <c r="B9" s="6">
-        <v>1</v>
-      </c>
-      <c r="C9" s="6">
-        <v>1</v>
-      </c>
-      <c r="D9" s="6">
-        <v>-1</v>
-      </c>
-      <c r="E9" s="6">
-        <v>1</v>
-      </c>
-      <c r="F9" s="6">
-        <v>-1</v>
-      </c>
-      <c r="G9" s="6">
-        <v>0</v>
-      </c>
-      <c r="H9" s="6">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3">
-        <v>0</v>
-      </c>
-      <c r="J9" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>1</v>
-      </c>
-      <c r="B10" s="6">
-        <v>-1</v>
-      </c>
-      <c r="C10" s="6">
-        <v>-1</v>
-      </c>
-      <c r="D10" s="6">
-        <v>-1</v>
-      </c>
-      <c r="E10" s="6">
-        <v>1</v>
-      </c>
-      <c r="F10" s="6">
-        <v>-1</v>
-      </c>
-      <c r="G10" s="6">
-        <v>0</v>
-      </c>
-      <c r="H10" s="6">
-        <v>-1</v>
-      </c>
-      <c r="I10" s="7">
-        <v>0</v>
-      </c>
-      <c r="J10" s="3">
-        <v>0</v>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1.5</v>
+      </c>
+      <c r="C1">
+        <v>1.5</v>
+      </c>
+      <c r="D1">
+        <v>0.5</v>
+      </c>
+      <c r="E1">
+        <v>1.5</v>
+      </c>
+      <c r="F1">
+        <v>0.5</v>
+      </c>
+      <c r="G1">
+        <v>1</v>
+      </c>
+      <c r="H1">
+        <v>0.5</v>
+      </c>
+      <c r="I1">
+        <v>0.5</v>
+      </c>
+      <c r="J1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0.5</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+      <c r="E2">
+        <v>1.5</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+      <c r="I2">
+        <v>0.5</v>
+      </c>
+      <c r="J2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0.5</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0.5</v>
+      </c>
+      <c r="E3">
+        <v>1.5</v>
+      </c>
+      <c r="F3">
+        <v>1.5</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0.5</v>
+      </c>
+      <c r="I3">
+        <v>0.5</v>
+      </c>
+      <c r="J3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1.5</v>
+      </c>
+      <c r="B4">
+        <v>1.5</v>
+      </c>
+      <c r="C4">
+        <v>1.5</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0.5</v>
+      </c>
+      <c r="F4">
+        <v>1.5</v>
+      </c>
+      <c r="G4">
+        <v>1.5</v>
+      </c>
+      <c r="H4">
+        <v>1.5</v>
+      </c>
+      <c r="I4">
+        <v>1.5</v>
+      </c>
+      <c r="J4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0.5</v>
+      </c>
+      <c r="B5">
+        <v>0.5</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>1.5</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1.5</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0.5</v>
+      </c>
+      <c r="I5">
+        <v>0.5</v>
+      </c>
+      <c r="J5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1.5</v>
+      </c>
+      <c r="B6">
+        <v>1.5</v>
+      </c>
+      <c r="C6">
+        <v>0.5</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+      <c r="E6">
+        <v>0.5</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1.5</v>
+      </c>
+      <c r="H6">
+        <v>1.5</v>
+      </c>
+      <c r="I6">
+        <v>1.5</v>
+      </c>
+      <c r="J6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0.5</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0.5</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1.5</v>
+      </c>
+      <c r="B8">
+        <v>1.5</v>
+      </c>
+      <c r="C8">
+        <v>1.5</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+      <c r="E8">
+        <v>1.5</v>
+      </c>
+      <c r="F8">
+        <v>0.5</v>
+      </c>
+      <c r="G8">
+        <v>1.5</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1.5</v>
+      </c>
+      <c r="B9">
+        <v>1.5</v>
+      </c>
+      <c r="C9">
+        <v>1.5</v>
+      </c>
+      <c r="D9">
+        <v>0.5</v>
+      </c>
+      <c r="E9">
+        <v>1.5</v>
+      </c>
+      <c r="F9">
+        <v>0.5</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1.5</v>
+      </c>
+      <c r="B10">
+        <v>0.5</v>
+      </c>
+      <c r="C10">
+        <v>0.5</v>
+      </c>
+      <c r="D10">
+        <v>0.5</v>
+      </c>
+      <c r="E10">
+        <v>1.5</v>
+      </c>
+      <c r="F10">
+        <v>0.5</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0.5</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited coefficients and finished line of reasoning
</commit_message>
<xml_diff>
--- a/main/MilitaryTactics.xlsx
+++ b/main/MilitaryTactics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\studentgvsc\Documents\Mentorship2020\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95F6BC1-F2B0-45F3-B5B1-89EC0D48E782}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE174CB-48AD-412D-9ED5-61BD0C36D450}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7980" yWindow="0" windowWidth="10590" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -268,7 +268,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -278,31 +278,31 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="C1">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
       <c r="D1">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="E1">
-        <v>1.5</v>
+        <v>1.61</v>
       </c>
       <c r="F1">
-        <v>0.5</v>
+        <v>0.44</v>
       </c>
       <c r="G1">
         <v>1</v>
       </c>
       <c r="H1">
-        <v>0.5</v>
+        <v>0.31</v>
       </c>
       <c r="I1">
-        <v>0.5</v>
+        <v>0.43</v>
       </c>
       <c r="J1">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>